<commit_message>
Spike Optimización manejo data ambiente Staging
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -8,13 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144022EE-CF72-4CE0-8070-641F313C5F56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DC1464-A3C8-4E58-AA95-DDB64A7EEF41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="821" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Retanqueo" sheetId="10" r:id="rId1"/>
-    <sheet name="ClientesBienvenidaRetanqueos" sheetId="1" r:id="rId2"/>
+    <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
+    <sheet name="AnalisisCreditoRetanqueo" sheetId="12" r:id="rId2"/>
+    <sheet name="ClientesBienvenidaRetanqueos" sheetId="13" r:id="rId3"/>
+    <sheet name="CreditosVisacionRetanqueos" sheetId="16" r:id="rId4"/>
+    <sheet name="DesembolsoRetanqueos" sheetId="14" r:id="rId5"/>
+    <sheet name="RetanqueoCCS" sheetId="15" r:id="rId6"/>
+    <sheet name="AnalisisCreditoRetanqueoCCS" sheetId="17" r:id="rId7"/>
+    <sheet name="ClientesBienvenidaRetanqueoCCS" sheetId="18" r:id="rId8"/>
+    <sheet name="CreditosVisacionRetanqueosCCS" sheetId="19" r:id="rId9"/>
+    <sheet name="DesembolsoCarteraCCS" sheetId="20" r:id="rId10"/>
+    <sheet name="VisacionSaneamientoCCS" sheetId="21" r:id="rId11"/>
+    <sheet name="DesembolsoSaneamientoCCS" sheetId="22" r:id="rId12"/>
+    <sheet name="DesembolsoRetanqueosCCS" sheetId="23" r:id="rId13"/>
+    <sheet name="RetanqueoMultiple" sheetId="10" r:id="rId14"/>
+    <sheet name="ClientesBienvenidaRetanqueoMult" sheetId="1" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="64">
   <si>
     <t>Cedula</t>
   </si>
@@ -58,32 +71,182 @@
     <t>TipoDesen</t>
   </si>
   <si>
-    <t>3125117715</t>
-  </si>
-  <si>
-    <t>prueba@mail.com</t>
-  </si>
-  <si>
-    <t>Efectivo</t>
-  </si>
-  <si>
-    <t>85863</t>
-  </si>
-  <si>
-    <t>1110448827</t>
-  </si>
-  <si>
-    <t>91216107</t>
-  </si>
-  <si>
-    <t>P.A COLPENSIONES</t>
+    <t>rutaPDF</t>
+  </si>
+  <si>
+    <t>Tasa</t>
+  </si>
+  <si>
+    <t>Plazo</t>
+  </si>
+  <si>
+    <t>DiasHabilesIntereses</t>
+  </si>
+  <si>
+    <t>Ingresos</t>
+  </si>
+  <si>
+    <t>descLey</t>
+  </si>
+  <si>
+    <t>descNomina</t>
+  </si>
+  <si>
+    <t>VlrCompraSaneamiento</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>"9000000"</t>
+  </si>
+  <si>
+    <t>"79919146"</t>
+  </si>
+  <si>
+    <t>"71403"</t>
+  </si>
+  <si>
+    <t>"src/test/resources/Data/PDFPRUEBA.pdf"</t>
+  </si>
+  <si>
+    <t>"90"</t>
+  </si>
+  <si>
+    <t>"10"</t>
+  </si>
+  <si>
+    <t>"6500000"</t>
+  </si>
+  <si>
+    <t>"380000"</t>
+  </si>
+  <si>
+    <t>"100000"</t>
+  </si>
+  <si>
+    <t>"3500000"</t>
+  </si>
+  <si>
+    <t>"2258"</t>
+  </si>
+  <si>
+    <t>"1.8"</t>
+  </si>
+  <si>
+    <t>NombreCredito</t>
+  </si>
+  <si>
+    <t>decLey</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>AnnoAfetacion</t>
+  </si>
+  <si>
+    <t>"WILLIAM FRANCISCO"</t>
+  </si>
+  <si>
+    <t>"Octubre"</t>
+  </si>
+  <si>
+    <t>"360000"</t>
+  </si>
+  <si>
+    <t>"19/10/2021"</t>
+  </si>
+  <si>
+    <t>"13"</t>
+  </si>
+  <si>
+    <t>"2021"</t>
+  </si>
+  <si>
+    <t>"3115128152"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Efectivo" </t>
+  </si>
+  <si>
+    <t>Banco</t>
+  </si>
+  <si>
+    <t>"Remanentes - 60237038927 - REMANENTE"</t>
+  </si>
+  <si>
+    <t>fechaActual</t>
+  </si>
+  <si>
+    <t>IngresosMes</t>
+  </si>
+  <si>
+    <t>"7000000"</t>
+  </si>
+  <si>
+    <t>"25"</t>
+  </si>
+  <si>
+    <t>"930000"</t>
+  </si>
+  <si>
+    <t>NombreCredio</t>
+  </si>
+  <si>
+    <t>Cartera1</t>
+  </si>
+  <si>
+    <t>Saneamiento2</t>
+  </si>
+  <si>
+    <t>"830000"</t>
+  </si>
+  <si>
+    <t>"Efectivo"</t>
+  </si>
+  <si>
+    <t>"24478657"</t>
+  </si>
+  <si>
+    <t>"1000000"</t>
+  </si>
+  <si>
+    <t>"dandresabogadog@mail.com"</t>
+  </si>
+  <si>
+    <t>"85863"</t>
+  </si>
+  <si>
+    <t>"1110448827"</t>
+  </si>
+  <si>
+    <t>"3125117715"</t>
+  </si>
+  <si>
+    <t>"5000000"</t>
+  </si>
+  <si>
+    <t>"91216107"</t>
+  </si>
+  <si>
+    <t>"P.A COLPENSIONES"</t>
+  </si>
+  <si>
+    <t>"71039"</t>
+  </si>
+  <si>
+    <t>"MARIA LUBIC"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +256,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -124,7 +294,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -405,11 +575,302 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAB8B06-AB93-4571-AE11-74C96A6F1D5F}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052627B-C391-4BA9-B8BF-A2F297901E10}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA008934-7A22-4614-999B-B2D834D4C993}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C31E397-96F1-4567-A47E-2ED291A7FBD7}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,13 +891,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1">
-        <v>5000000</v>
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -444,17 +905,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="30.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -476,26 +939,633 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{9840C493-B129-4F1C-B7EA-9D2CB891C77A}"/>
+    <hyperlink ref="D2" r:id="rId1" display="dandresabogadog@mail.com" xr:uid="{E0D8C32B-A6F8-4EF6-A36F-73FC45FA7DC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEB2DC1-DD13-4EE2-AF82-4D7C753944BA}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB72DA3-A450-4417-B142-66D79AC54194}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="dandresabogadog@mail.com" xr:uid="{28177C8A-F863-40DF-8E14-D555DE197E55}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD989E4E-BFC5-4F53-901F-526EE94C831B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FF4E62-774D-4D01-9FBA-7F8FE9345C86}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4867155A-9367-4611-B57D-923A3BAD7224}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D03B82-94E7-48A9-A335-0AAF3C0935B9}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A8EF61-4AD7-4161-AFD3-D7038E375362}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="dandresabogadog@mail.com" xr:uid="{5372925A-5B01-4F55-AC86-8B7393ADE141}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B23121-DCE4-41C0-BE42-84D85AC5DB0E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Generalizar data retanqueo en el excel
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61606D2-675F-4702-9810-01993B5A8363}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3D6A8E-F836-49C9-806F-990364F61333}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -234,12 +234,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -255,10 +261,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -553,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,34 +590,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K1" t="s">
@@ -618,16 +626,16 @@
       <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>27</v>
       </c>
       <c r="Q1" t="s">
@@ -723,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4867155A-9367-4611-B57D-923A3BAD7224}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,58 +762,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="3" t="s">
         <v>38</v>
       </c>
       <c r="S1" t="s">
@@ -817,7 +825,7 @@
       <c r="U1" t="s">
         <v>6</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="3" t="s">
         <v>35</v>
       </c>
       <c r="W1" t="s">
@@ -911,7 +919,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,16 +933,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">

</xml_diff>

<commit_message>
Archivo con modificacion para retanqeo Multiple
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3D6A8E-F836-49C9-806F-990364F61333}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9348BA5-ECCA-490F-B052-1B2B9A48955C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
   <si>
     <t>Cedula</t>
   </si>
@@ -173,9 +173,6 @@
     <t>"5000000"</t>
   </si>
   <si>
-    <t>"91216107"</t>
-  </si>
-  <si>
     <t>"P.A COLPENSIONES"</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>"3145363053"</t>
+  </si>
+  <si>
+    <t>"8682110"</t>
   </si>
 </sst>
 </file>
@@ -261,18 +261,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -561,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,13 +668,13 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -686,19 +698,19 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
@@ -713,7 +725,7 @@
         <v>32</v>
       </c>
       <c r="T2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U2" t="s">
         <v>34</v>
@@ -732,7 +744,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,13 +846,13 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -870,13 +882,13 @@
         <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
@@ -885,10 +897,10 @@
         <v>21</v>
       </c>
       <c r="R2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" t="s">
         <v>54</v>
-      </c>
-      <c r="S2" t="s">
-        <v>55</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>41</v>
@@ -897,7 +909,7 @@
         <v>40</v>
       </c>
       <c r="V2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W2" t="s">
         <v>34</v>
@@ -905,7 +917,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="T2" r:id="rId1" display="dandresabogadog@mail.com" xr:uid="{5372925A-5B01-4F55-AC86-8B7393ADE141}"/>
@@ -916,10 +928,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +944,7 @@
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -954,16 +966,43 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>42</v>
@@ -977,13 +1016,42 @@
       <c r="G2" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <conditionalFormatting sqref="H1:H2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="dandresabogadog@mail.com" xr:uid="{E0D8C32B-A6F8-4EF6-A36F-73FC45FA7DC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pantalla simulador analista  - Retanqueo multiple
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9348BA5-ECCA-490F-B052-1B2B9A48955C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A9D716-8388-46A7-B517-DB503FAD5EE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="58">
   <si>
     <t>Cedula</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>"8682110"</t>
+  </si>
+  <si>
+    <t>"25/10/2021"</t>
+  </si>
+  <si>
+    <t>"LUIS CARLOS"</t>
   </si>
 </sst>
 </file>
@@ -928,23 +934,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -993,8 +1016,32 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -1042,6 +1089,30 @@
       </c>
       <c r="P2" t="s">
         <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" t="s">
+        <v>56</v>
+      </c>
+      <c r="V2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios retanqueo multiple, simulador interno
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A9D716-8388-46A7-B517-DB503FAD5EE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F5FDF2-6C55-4EA1-95BF-E84EBFCF5E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -173,9 +173,6 @@
     <t>"5000000"</t>
   </si>
   <si>
-    <t>"P.A COLPENSIONES"</t>
-  </si>
-  <si>
     <t>"24580532"</t>
   </si>
   <si>
@@ -203,13 +200,16 @@
     <t>"3145363053"</t>
   </si>
   <si>
-    <t>"8682110"</t>
-  </si>
-  <si>
     <t>"25/10/2021"</t>
   </si>
   <si>
-    <t>"LUIS CARLOS"</t>
+    <t>"27072341"</t>
+  </si>
+  <si>
+    <t>"FOPEP"</t>
+  </si>
+  <si>
+    <t>"ALBA  DE JESUS"</t>
   </si>
 </sst>
 </file>
@@ -674,13 +674,13 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -704,19 +704,19 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
@@ -731,7 +731,7 @@
         <v>32</v>
       </c>
       <c r="T2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U2" t="s">
         <v>34</v>
@@ -852,13 +852,13 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -888,13 +888,13 @@
         <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
@@ -903,10 +903,10 @@
         <v>21</v>
       </c>
       <c r="R2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" t="s">
         <v>53</v>
-      </c>
-      <c r="S2" t="s">
-        <v>54</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>41</v>
@@ -915,7 +915,7 @@
         <v>40</v>
       </c>
       <c r="V2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W2" t="s">
         <v>34</v>
@@ -936,14 +936,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -1049,7 +1048,7 @@
         <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>42</v>
@@ -1085,7 +1084,7 @@
         <v>21</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -1097,22 +1096,22 @@
         <v>28</v>
       </c>
       <c r="S2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T2" t="s">
         <v>30</v>
       </c>
       <c r="U2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V2" t="s">
         <v>34</v>
       </c>
       <c r="W2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios simulador analista, Retanqueo Múltiple
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F5FDF2-6C55-4EA1-95BF-E84EBFCF5E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCCFCDA-E9D2-4306-BFF4-0482830F43DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,13 +203,13 @@
     <t>"25/10/2021"</t>
   </si>
   <si>
-    <t>"27072341"</t>
+    <t>"12962960"</t>
   </si>
   <si>
     <t>"FOPEP"</t>
   </si>
   <si>
-    <t>"ALBA  DE JESUS"</t>
+    <t>"ROBERTO HERNAN"</t>
   </si>
 </sst>
 </file>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Retanqueo multiple analisis de credito CCS
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCCFCDA-E9D2-4306-BFF4-0482830F43DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1AB537-CFD1-4DCD-AAA0-06343F10C90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,13 +203,13 @@
     <t>"25/10/2021"</t>
   </si>
   <si>
-    <t>"12962960"</t>
-  </si>
-  <si>
-    <t>"FOPEP"</t>
-  </si>
-  <si>
-    <t>"ROBERTO HERNAN"</t>
+    <t>"JHON FREDY"</t>
+  </si>
+  <si>
+    <t>"10002426"</t>
+  </si>
+  <si>
+    <t>"P.A COLPENSIONES"</t>
   </si>
 </sst>
 </file>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>42</v>
@@ -1084,13 +1084,13 @@
         <v>21</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R2" t="s">
         <v>28</v>
@@ -1108,10 +1108,10 @@
         <v>34</v>
       </c>
       <c r="W2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="X2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simulador Analista validaciones compra cartera - saneamiento retanqueo múltiple
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1AB537-CFD1-4DCD-AAA0-06343F10C90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BB0DDB-E5B6-4C8E-B7C3-3C08D6CD9BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -203,13 +203,13 @@
     <t>"25/10/2021"</t>
   </si>
   <si>
-    <t>"JHON FREDY"</t>
-  </si>
-  <si>
-    <t>"10002426"</t>
-  </si>
-  <si>
-    <t>"P.A COLPENSIONES"</t>
+    <t>"34957577"</t>
+  </si>
+  <si>
+    <t>"FOPEP"</t>
+  </si>
+  <si>
+    <t>"EMMA LUCILA"</t>
   </si>
 </sst>
 </file>
@@ -936,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>42</v>
@@ -1090,7 +1090,7 @@
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="R2" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Ajuste Retanqueo (Carteras) - Digicredito
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4595C1E9-B42D-48EA-BA31-0EC3F80A9E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922E3611-C58B-4463-A7EC-9B1D282F7516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="15" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="74">
   <si>
     <t>Cedula</t>
   </si>
@@ -244,7 +244,22 @@
     <t>"300000"</t>
   </si>
   <si>
-    <t>""</t>
+    <t>"134950"</t>
+  </si>
+  <si>
+    <t>"200000"</t>
+  </si>
+  <si>
+    <t>"450000"</t>
+  </si>
+  <si>
+    <t>"3228483385"</t>
+  </si>
+  <si>
+    <t>"25/11/2021"</t>
+  </si>
+  <si>
+    <t>"86308"</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1345,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,10 +1429,10 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1426,28 +1441,28 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
@@ -1459,13 +1474,13 @@
         <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="R2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="S2" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>41</v>
@@ -1474,13 +1489,13 @@
         <v>40</v>
       </c>
       <c r="V2" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="W2" t="s">
         <v>34</v>
       </c>
       <c r="X2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flujo retanqueo digicredito con compra cartera
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D92792-A23D-4646-96AB-DDF5EB8D1D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE2499D-08B8-49D6-9E0B-7E7B3AE664B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" tabRatio="821" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -259,7 +259,7 @@
     <t>"25/11/2021"</t>
   </si>
   <si>
-    <t>"86308"</t>
+    <t>"86318"</t>
   </si>
 </sst>
 </file>
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4941B7E2-706E-4D94-84AC-BEDA7D2028C7}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ajuste Mostrar Campos Fianza - simulador interno, Ajuste Mostrar Campos Fianza - Llamada de bienvenida, Ajuste Mostrar Campos Fianza - simulador analista
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F609226-DD82-47E0-AB31-732986D9D99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED13017C-FE5B-4311-B601-FCC7CD27B85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="76">
   <si>
     <t>Cedula</t>
   </si>
@@ -175,30 +175,18 @@
     <t>"5000000"</t>
   </si>
   <si>
-    <t>"24580532"</t>
-  </si>
-  <si>
-    <t>"78635"</t>
-  </si>
-  <si>
     <t>"8000000"</t>
   </si>
   <si>
     <t>"0"</t>
   </si>
   <si>
-    <t>"BLANCA NURY"</t>
-  </si>
-  <si>
     <t>"14/06/1969"</t>
   </si>
   <si>
     <t>"20/10/2021"</t>
   </si>
   <si>
-    <t>"730000"</t>
-  </si>
-  <si>
     <t>"3145363053"</t>
   </si>
   <si>
@@ -260,6 +248,24 @@
   </si>
   <si>
     <t>"86379"</t>
+  </si>
+  <si>
+    <t>"Diciembre"</t>
+  </si>
+  <si>
+    <t>"9696579"</t>
+  </si>
+  <si>
+    <t>"MANUEL ERACLIO"</t>
+  </si>
+  <si>
+    <t>"72949"</t>
+  </si>
+  <si>
+    <t>"1030000"</t>
+  </si>
+  <si>
+    <t>"14/12/2021"</t>
   </si>
 </sst>
 </file>
@@ -640,7 +646,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,13 +740,13 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -764,19 +770,19 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
@@ -791,7 +797,7 @@
         <v>32</v>
       </c>
       <c r="T2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="U2" t="s">
         <v>34</v>
@@ -809,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4867155A-9367-4611-B57D-923A3BAD7224}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,13 +918,13 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -945,28 +951,28 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="M2" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="R2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="S2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>41</v>
@@ -975,7 +981,7 @@
         <v>40</v>
       </c>
       <c r="V2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="W2" t="s">
         <v>34</v>
@@ -1102,13 +1108,13 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>42</v>
@@ -1144,34 +1150,34 @@
         <v>21</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="R2" t="s">
         <v>28</v>
       </c>
       <c r="S2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="T2" t="s">
         <v>30</v>
       </c>
       <c r="U2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="V2" t="s">
         <v>34</v>
       </c>
       <c r="W2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="X2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1190,7 +1196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD10BD7-2917-47E9-9904-E83A367B63F9}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1261,18 +1267,18 @@
         <v>33</v>
       </c>
       <c r="V1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1281,34 +1287,34 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
@@ -1323,13 +1329,13 @@
         <v>32</v>
       </c>
       <c r="T2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="U2" t="s">
         <v>34</v>
       </c>
       <c r="V2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1421,18 +1427,18 @@
         <v>33</v>
       </c>
       <c r="X1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1441,46 +1447,46 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
         <v>64</v>
       </c>
-      <c r="I2" t="s">
-        <v>68</v>
-      </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="R2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="S2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>41</v>
@@ -1489,13 +1495,13 @@
         <v>40</v>
       </c>
       <c r="V2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="W2" t="s">
         <v>34</v>
       </c>
       <c r="X2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validacion dinamicas contables Retanqueo Mensualizado - Anticipado
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\ana.desarrollo59\Documents\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6CAFF8-C74D-4E0F-AB07-40BEC37EDBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22884F04-287F-4BA9-81A5-5129A60C8589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -575,6 +575,157 @@
         </r>
       </text>
     </comment>
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{A37D49B0-89A6-4035-8531-C50855960E53}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Consultar usos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{F740A4AF-2CD8-49B0-B055-FBC38636073D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Consultar usos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{DDE583A6-D61C-4F2D-90C9-BE29FC30CBA9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Consultar usos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{92199678-7173-4012-A34B-8C2B07EE3CC1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Consultar usos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{E1F9D26A-EEEB-4D01-B250-214CA0C9A913}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fecha en la cual se genera el registro del Cliente.
+Fecha Actual
+*Formato;
+DD/MM/AA
+*Mes formato digital.
+*Dia menor a 10 anteponer Cero.
+*Año completo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{6877FF6D-2E25-44A6-9EBC-7825958A73FA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Numero de radicación de la solicitud.
+Consultarlo en base de datos.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -2973,7 +3124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="104">
   <si>
     <t>Cedula</t>
   </si>
@@ -3101,21 +3252,12 @@
     <t>"5000000"</t>
   </si>
   <si>
-    <t>"24580532"</t>
-  </si>
-  <si>
-    <t>"78635"</t>
-  </si>
-  <si>
     <t>"8000000"</t>
   </si>
   <si>
     <t>"0"</t>
   </si>
   <si>
-    <t>"BLANCA NURY"</t>
-  </si>
-  <si>
     <t>"14/06/1969"</t>
   </si>
   <si>
@@ -3225,6 +3367,75 @@
   </si>
   <si>
     <t>"1.80"</t>
+  </si>
+  <si>
+    <t>"20000000"</t>
+  </si>
+  <si>
+    <t>"1.70"</t>
+  </si>
+  <si>
+    <t>"120"</t>
+  </si>
+  <si>
+    <t>"3204992496"</t>
+  </si>
+  <si>
+    <t>"jvcutilidades@hotmail.com"</t>
+  </si>
+  <si>
+    <t>"19/01/2022"</t>
+  </si>
+  <si>
+    <t>"30"</t>
+  </si>
+  <si>
+    <t>"03/09/1967"</t>
+  </si>
+  <si>
+    <t>FechaRegistro</t>
+  </si>
+  <si>
+    <t>NumRadicado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"'ACRED','EGRESO'" </t>
+  </si>
+  <si>
+    <t>"upper('Desembolso egreso'), upper('Desembolso activación de crédito')"</t>
+  </si>
+  <si>
+    <t>AccountingSourcePadre</t>
+  </si>
+  <si>
+    <t>AccountingNamePadre</t>
+  </si>
+  <si>
+    <t>AccountingSourceHijo</t>
+  </si>
+  <si>
+    <t>AccountingNameHijo</t>
+  </si>
+  <si>
+    <t>"upper('Retanqueo de créditos')"</t>
+  </si>
+  <si>
+    <t>19/01/2022</t>
+  </si>
+  <si>
+    <t>"'RETANQ'"</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>"74751"</t>
+  </si>
+  <si>
+    <t>"11299956"</t>
+  </si>
+  <si>
+    <t>"ÁLFREDO CARVAJAL"</t>
   </si>
 </sst>
 </file>
@@ -3308,7 +3519,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
@@ -3324,13 +3535,35 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3847,10 +4080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3866,18 +4099,24 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22" customWidth="1"/>
+    <col min="23" max="23" width="33.140625" customWidth="1"/>
+    <col min="24" max="24" width="24.5703125" customWidth="1"/>
+    <col min="25" max="25" width="67.5703125" customWidth="1"/>
+    <col min="26" max="26" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3941,84 +4180,124 @@
       <c r="U1" t="s">
         <v>31</v>
       </c>
+      <c r="V1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="Q2" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="S2" t="s">
         <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>32</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:F2">
+    <cfRule type="duplicateValues" dxfId="24" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:J2">
     <cfRule type="duplicateValues" dxfId="23" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:J2">
-    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
+  <conditionalFormatting sqref="V1:AA2">
+    <cfRule type="duplicateValues" dxfId="22" priority="13"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" display="dandresabogadog@mail.com" xr:uid="{8C69726B-A170-403B-85D4-861645813F44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4127,28 +4406,28 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>20</v>
@@ -4160,28 +4439,28 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" t="s">
         <v>73</v>
       </c>
-      <c r="M2" t="s">
-        <v>80</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>74</v>
       </c>
-      <c r="O2" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>76</v>
-      </c>
-      <c r="R2" t="s">
-        <v>77</v>
-      </c>
       <c r="S2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>38</v>
@@ -4190,7 +4469,7 @@
         <v>37</v>
       </c>
       <c r="V2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>32</v>
@@ -4341,13 +4620,13 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
@@ -4365,7 +4644,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>17</v>
@@ -4383,34 +4662,34 @@
         <v>21</v>
       </c>
       <c r="O2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R2" t="s">
         <v>27</v>
       </c>
       <c r="S2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="T2" t="s">
         <v>28</v>
       </c>
       <c r="U2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="W2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="X2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -4543,54 +4822,54 @@
         <v>31</v>
       </c>
       <c r="V1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P2" t="s">
         <v>28</v>
@@ -4605,13 +4884,13 @@
         <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="V2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -4736,66 +5015,66 @@
         <v>31</v>
       </c>
       <c r="X1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P2" t="s">
         <v>28</v>
       </c>
       <c r="Q2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="R2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>38</v>
@@ -4804,13 +5083,13 @@
         <v>37</v>
       </c>
       <c r="V2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="X2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
commit para solucionar error de xpath en confirmar carteras
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\ana.desarrollo59\Documents\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22884F04-287F-4BA9-81A5-5129A60C8589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F812B4C8-A853-4CD0-A857-96F568C6CF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{21B08E5A-6B45-4269-9207-ECD196F8BCD2}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{3A015C19-3CC0-4138-9366-0C710DE03CF0}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{E0B704B7-E349-4310-A7B4-8B013DD1A588}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{EC3515F5-9680-47C9-8F92-F4C8CF501498}">
       <text>
         <r>
           <rPr>
@@ -343,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{6B673BA1-244E-44B6-958C-6EC049E9A42C}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{BB1F52AD-6BDA-4E36-A209-5C5043E7831E}">
       <text>
         <r>
           <rPr>
@@ -1833,31 +1833,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{E3E59771-6B0D-4E31-B827-6201EB56B990}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{3D122B94-6A4C-49B8-A8B8-A39C8596D0DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fecha en la cual se genera el registro del Cliente.
 Fecha Actual
-*Formato de fecha:
+*Formato;
 DD/MM/AA
-*Mes en formato alfabético, solo tres primeras letras, inicial en mayúscula
-*Dia menor a 10 inicia por Cero</t>
+*Mes formato digital.
+*Dia menor a 10 anteponer Cero.
+*Año completo</t>
         </r>
       </text>
     </comment>
@@ -3267,18 +3269,6 @@
     <t>"3145363053"</t>
   </si>
   <si>
-    <t>"25/10/2021"</t>
-  </si>
-  <si>
-    <t>"12962960"</t>
-  </si>
-  <si>
-    <t>"FOPEP"</t>
-  </si>
-  <si>
-    <t>"ROBERTO HERNAN"</t>
-  </si>
-  <si>
     <t>NumRadicadoCredito</t>
   </si>
   <si>
@@ -3351,15 +3341,6 @@
     <t>"430000"</t>
   </si>
   <si>
-    <t>"93341535"</t>
-  </si>
-  <si>
-    <t>"83108"</t>
-  </si>
-  <si>
-    <t>"ALEXANDER"</t>
-  </si>
-  <si>
     <t>"1.60"</t>
   </si>
   <si>
@@ -3420,22 +3401,43 @@
     <t>"upper('Retanqueo de créditos')"</t>
   </si>
   <si>
-    <t>19/01/2022</t>
-  </si>
-  <si>
     <t>"'RETANQ'"</t>
   </si>
   <si>
     <t>null</t>
   </si>
   <si>
-    <t>"74751"</t>
-  </si>
-  <si>
-    <t>"11299956"</t>
-  </si>
-  <si>
-    <t>"ÁLFREDO CARVAJAL"</t>
+    <t>"7505895"</t>
+  </si>
+  <si>
+    <t>"52975"</t>
+  </si>
+  <si>
+    <t>"Camilo"</t>
+  </si>
+  <si>
+    <t>"24/01/2022"</t>
+  </si>
+  <si>
+    <t>"Bancolombia Remanentes - 60237038927 - REMANENTE"</t>
+  </si>
+  <si>
+    <t>"25/01/2022"</t>
+  </si>
+  <si>
+    <t>"400000"</t>
+  </si>
+  <si>
+    <t>"600000"</t>
+  </si>
+  <si>
+    <t>"P.A COLPENSIONES"</t>
+  </si>
+  <si>
+    <t>"10157598"</t>
+  </si>
+  <si>
+    <t>"AMADEO"</t>
   </si>
 </sst>
 </file>
@@ -4082,8 +4084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4181,51 +4183,51 @@
         <v>31</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="Z1" s="11" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>21</v>
@@ -4237,49 +4239,49 @@
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="N2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="O2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Q2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="S2" t="s">
         <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="Y2" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA2" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="Z2" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4305,7 +4307,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4867155A-9367-4611-B57D-923A3BAD7224}">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4406,28 +4410,28 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>20</v>
@@ -4439,25 +4443,25 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="N2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="O2" t="s">
         <v>44</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Q2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="R2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="S2" t="s">
         <v>46</v>
@@ -4469,7 +4473,7 @@
         <v>37</v>
       </c>
       <c r="V2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>32</v>
@@ -4513,9 +4517,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4620,13 +4626,13 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
@@ -4644,7 +4650,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>17</v>
@@ -4662,16 +4668,16 @@
         <v>21</v>
       </c>
       <c r="O2" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="R2" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="S2" t="s">
         <v>44</v>
@@ -4679,43 +4685,31 @@
       <c r="T2" t="s">
         <v>28</v>
       </c>
-      <c r="U2" t="s">
-        <v>47</v>
+      <c r="U2" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="W2" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="X2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="I2:J2">
     <cfRule type="duplicateValues" dxfId="12" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J2">
+  <conditionalFormatting sqref="K2:N2">
     <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:N2">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+  <conditionalFormatting sqref="U2">
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="dandresabogadog@mail.com" xr:uid="{A2E15BB9-0155-4310-87D2-2FBC767C3147}"/>
@@ -4822,39 +4816,39 @@
         <v>31</v>
       </c>
       <c r="V1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K2" t="s">
         <v>43</v>
@@ -4863,7 +4857,7 @@
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
@@ -4890,7 +4884,7 @@
         <v>32</v>
       </c>
       <c r="V2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -5015,7 +5009,7 @@
         <v>31</v>
       </c>
       <c r="X1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -5023,40 +5017,40 @@
         <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
@@ -5068,13 +5062,13 @@
         <v>28</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="R2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="S2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>38</v>
@@ -5083,13 +5077,13 @@
         <v>37</v>
       </c>
       <c r="V2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="X2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Flujo validación dinámicas retanqueo multiple
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\ana.desarrollo59\Documents\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22884F04-287F-4BA9-81A5-5129A60C8589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56DE76C-99D9-41C9-9C98-A8DDE0B26E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{21B08E5A-6B45-4269-9207-ECD196F8BCD2}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{3A015C19-3CC0-4138-9366-0C710DE03CF0}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{E0B704B7-E349-4310-A7B4-8B013DD1A588}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{EC3515F5-9680-47C9-8F92-F4C8CF501498}">
       <text>
         <r>
           <rPr>
@@ -343,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{6B673BA1-244E-44B6-958C-6EC049E9A42C}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{BB1F52AD-6BDA-4E36-A209-5C5043E7831E}">
       <text>
         <r>
           <rPr>
@@ -1833,31 +1833,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{E3E59771-6B0D-4E31-B827-6201EB56B990}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{3D122B94-6A4C-49B8-A8B8-A39C8596D0DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fecha en la cual se genera el registro del Cliente.
 Fecha Actual
-*Formato de fecha:
+*Formato;
 DD/MM/AA
-*Mes en formato alfabético, solo tres primeras letras, inicial en mayúscula
-*Dia menor a 10 inicia por Cero</t>
+*Mes formato digital.
+*Dia menor a 10 anteponer Cero.
+*Año completo</t>
         </r>
       </text>
     </comment>
@@ -1932,6 +1934,110 @@
           <t xml:space="preserve">
 Monto del Saneamiento que se va a recoger;
 *No debe tener puntos ni comas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{D7194442-9A4A-4145-B7A0-D80CA6E92F4C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mes en el cual se va a lanzar la Originación;
+*Siempre mes Actual
+*Mes Escrito Completo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{9C5E7FBC-409D-40E7-AED5-5945C41A6D18}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mes en el cual se va a lanzar la Originación;
+*Siempre mes Actual
+*Mes Escrito Completo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{78480628-1E1A-4E4C-9099-1438A7A9F5A3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mes en el cual se va a lanzar la Originación;
+*Siempre mes Actual
+*Mes Escrito Completo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{995885CC-2A77-4317-B13A-66EC69C04D39}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mes en el cual se va a lanzar la Originación;
+*Siempre mes Actual
+*Mes Escrito Completo</t>
         </r>
       </text>
     </comment>
@@ -3124,7 +3230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="106">
   <si>
     <t>Cedula</t>
   </si>
@@ -3249,9 +3355,6 @@
     <t>"3125117715"</t>
   </si>
   <si>
-    <t>"5000000"</t>
-  </si>
-  <si>
     <t>"8000000"</t>
   </si>
   <si>
@@ -3267,18 +3370,6 @@
     <t>"3145363053"</t>
   </si>
   <si>
-    <t>"25/10/2021"</t>
-  </si>
-  <si>
-    <t>"12962960"</t>
-  </si>
-  <si>
-    <t>"FOPEP"</t>
-  </si>
-  <si>
-    <t>"ROBERTO HERNAN"</t>
-  </si>
-  <si>
     <t>NumRadicadoCredito</t>
   </si>
   <si>
@@ -3351,15 +3442,6 @@
     <t>"430000"</t>
   </si>
   <si>
-    <t>"93341535"</t>
-  </si>
-  <si>
-    <t>"83108"</t>
-  </si>
-  <si>
-    <t>"ALEXANDER"</t>
-  </si>
-  <si>
     <t>"1.60"</t>
   </si>
   <si>
@@ -3420,22 +3502,52 @@
     <t>"upper('Retanqueo de créditos')"</t>
   </si>
   <si>
-    <t>19/01/2022</t>
-  </si>
-  <si>
     <t>"'RETANQ'"</t>
   </si>
   <si>
     <t>null</t>
   </si>
   <si>
-    <t>"74751"</t>
-  </si>
-  <si>
-    <t>"11299956"</t>
-  </si>
-  <si>
-    <t>"ÁLFREDO CARVAJAL"</t>
+    <t>"7505895"</t>
+  </si>
+  <si>
+    <t>"52975"</t>
+  </si>
+  <si>
+    <t>"Camilo"</t>
+  </si>
+  <si>
+    <t>"24/01/2022"</t>
+  </si>
+  <si>
+    <t>"Bancolombia Remanentes - 60237038927 - REMANENTE"</t>
+  </si>
+  <si>
+    <t>"P.A COLPENSIONES"</t>
+  </si>
+  <si>
+    <t>"'upper('Desembolso egreso'), upper('Desembolso activación de crédito')'"</t>
+  </si>
+  <si>
+    <t>"'ACRED','EGRESO'''</t>
+  </si>
+  <si>
+    <t>"01/02/2022"</t>
+  </si>
+  <si>
+    <t>"10000000"</t>
+  </si>
+  <si>
+    <t>"10160945"</t>
+  </si>
+  <si>
+    <t>"Orlando"</t>
+  </si>
+  <si>
+    <t>"08/07/1952"</t>
+  </si>
+  <si>
+    <t>"Febrero"</t>
   </si>
 </sst>
 </file>
@@ -3519,7 +3631,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
@@ -3547,6 +3659,7 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -4082,8 +4195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4181,105 +4294,105 @@
         <v>31</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="11" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="N2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="O2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="S2" t="s">
         <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="X2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA2" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z2" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4305,7 +4418,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4867155A-9367-4611-B57D-923A3BAD7224}">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4406,28 +4521,28 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>20</v>
@@ -4439,28 +4554,28 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="N2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="S2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>38</v>
@@ -4469,7 +4584,7 @@
         <v>37</v>
       </c>
       <c r="V2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>32</v>
@@ -4513,9 +4628,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4542,9 +4659,10 @@
     <col min="22" max="22" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4617,16 +4735,34 @@
       <c r="X1" t="s">
         <v>36</v>
       </c>
+      <c r="Y1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
@@ -4644,7 +4780,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>17</v>
@@ -4662,60 +4798,66 @@
         <v>21</v>
       </c>
       <c r="O2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="R2" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="S2" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="T2" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" t="s">
-        <v>47</v>
+        <v>67</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="W2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD2" s="15" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="I2:J2">
     <cfRule type="duplicateValues" dxfId="12" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J2">
+  <conditionalFormatting sqref="K2:N2">
     <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:N2">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+  <conditionalFormatting sqref="U2">
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="dandresabogadog@mail.com" xr:uid="{A2E15BB9-0155-4310-87D2-2FBC767C3147}"/>
@@ -4822,54 +4964,54 @@
         <v>31</v>
       </c>
       <c r="V1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P2" t="s">
         <v>28</v>
@@ -4884,13 +5026,13 @@
         <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="V2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -5015,66 +5157,66 @@
         <v>31</v>
       </c>
       <c r="X1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P2" t="s">
         <v>28</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="R2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" t="s">
         <v>59</v>
-      </c>
-      <c r="S2" t="s">
-        <v>64</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>38</v>
@@ -5083,13 +5225,13 @@
         <v>37</v>
       </c>
       <c r="V2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="X2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Validación dinámicas contables retanqueo multiple y ajuste función retanqueo
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56DE76C-99D9-41C9-9C98-A8DDE0B26E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5EFD6F-5294-43B3-8D01-45F80679F36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -3230,7 +3230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="107">
   <si>
     <t>Cedula</t>
   </si>
@@ -3451,30 +3451,15 @@
     <t>"1.80"</t>
   </si>
   <si>
-    <t>"20000000"</t>
-  </si>
-  <si>
     <t>"1.70"</t>
   </si>
   <si>
     <t>"120"</t>
   </si>
   <si>
-    <t>"3204992496"</t>
-  </si>
-  <si>
-    <t>"jvcutilidades@hotmail.com"</t>
-  </si>
-  <si>
-    <t>"19/01/2022"</t>
-  </si>
-  <si>
     <t>"30"</t>
   </si>
   <si>
-    <t>"03/09/1967"</t>
-  </si>
-  <si>
     <t>FechaRegistro</t>
   </si>
   <si>
@@ -3517,15 +3502,9 @@
     <t>"Camilo"</t>
   </si>
   <si>
-    <t>"24/01/2022"</t>
-  </si>
-  <si>
     <t>"Bancolombia Remanentes - 60237038927 - REMANENTE"</t>
   </si>
   <si>
-    <t>"P.A COLPENSIONES"</t>
-  </si>
-  <si>
     <t>"'upper('Desembolso egreso'), upper('Desembolso activación de crédito')'"</t>
   </si>
   <si>
@@ -3535,19 +3514,43 @@
     <t>"01/02/2022"</t>
   </si>
   <si>
-    <t>"10000000"</t>
-  </si>
-  <si>
-    <t>"10160945"</t>
-  </si>
-  <si>
-    <t>"Orlando"</t>
-  </si>
-  <si>
-    <t>"08/07/1952"</t>
-  </si>
-  <si>
     <t>"Febrero"</t>
+  </si>
+  <si>
+    <t>"5000000"</t>
+  </si>
+  <si>
+    <t>"JOSE ALBEIRO"</t>
+  </si>
+  <si>
+    <t>"10112372"</t>
+  </si>
+  <si>
+    <t>"P.A. FIDUPREVISORA NÓMINA PENSIONADOS FOMAG"</t>
+  </si>
+  <si>
+    <t>"20/07/1963"</t>
+  </si>
+  <si>
+    <t>"aalvarez@excelcredit.co"</t>
+  </si>
+  <si>
+    <t>"05/05/1945"</t>
+  </si>
+  <si>
+    <t>"3183903022"</t>
+  </si>
+  <si>
+    <t>"13951080"</t>
+  </si>
+  <si>
+    <t>"56530"</t>
+  </si>
+  <si>
+    <t>"07/02/2022"</t>
+  </si>
+  <si>
+    <t>"HERNANDO"</t>
   </si>
 </sst>
 </file>
@@ -4195,8 +4198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4294,45 +4297,45 @@
         <v>31</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Z1" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>19</v>
@@ -4350,49 +4353,49 @@
         <v>22</v>
       </c>
       <c r="M2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2" t="s">
         <v>94</v>
       </c>
-      <c r="N2" t="s">
-        <v>66</v>
-      </c>
       <c r="O2" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="P2" t="s">
         <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="S2" t="s">
         <v>30</v>
       </c>
       <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="X2" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="U2" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="Y2" s="12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="Z2" s="13" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -4524,10 +4527,10 @@
         <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -4557,7 +4560,7 @@
         <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="N2" t="s">
         <v>66</v>
@@ -4630,8 +4633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4660,6 +4663,7 @@
     <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -4736,33 +4740,33 @@
         <v>36</v>
       </c>
       <c r="Y1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="Z1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="AA1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="AB1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="AC1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="AD1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
@@ -4804,22 +4808,22 @@
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="R2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="S2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="T2" t="s">
         <v>67</v>
       </c>
       <c r="U2" s="13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="W2" t="s">
         <v>42</v>
@@ -4828,22 +4832,22 @@
         <v>42</v>
       </c>
       <c r="Y2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="Z2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="AA2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="AB2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="AC2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AD2" s="15" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validación proyección de saldo al día
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5EFD6F-5294-43B3-8D01-45F80679F36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6050CCF4-F5A9-49C1-8E2B-8654367EE9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -3520,18 +3520,6 @@
     <t>"5000000"</t>
   </si>
   <si>
-    <t>"JOSE ALBEIRO"</t>
-  </si>
-  <si>
-    <t>"10112372"</t>
-  </si>
-  <si>
-    <t>"P.A. FIDUPREVISORA NÓMINA PENSIONADOS FOMAG"</t>
-  </si>
-  <si>
-    <t>"20/07/1963"</t>
-  </si>
-  <si>
     <t>"aalvarez@excelcredit.co"</t>
   </si>
   <si>
@@ -3551,6 +3539,18 @@
   </si>
   <si>
     <t>"HERNANDO"</t>
+  </si>
+  <si>
+    <t>"P.A COLPENSIONES"</t>
+  </si>
+  <si>
+    <t>"12960211"</t>
+  </si>
+  <si>
+    <t>"GERARDO BENJAMIN"</t>
+  </si>
+  <si>
+    <t>"05/03/2022"</t>
   </si>
 </sst>
 </file>
@@ -4198,7 +4198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -4320,10 +4320,10 @@
         <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -4353,28 +4353,28 @@
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N2" t="s">
         <v>94</v>
       </c>
       <c r="O2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="P2" t="s">
         <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="S2" t="s">
         <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>90</v>
@@ -4392,7 +4392,7 @@
         <v>79</v>
       </c>
       <c r="Z2" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>86</v>
@@ -4633,8 +4633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4760,13 +4760,13 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
@@ -4784,7 +4784,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>17</v>
@@ -4808,13 +4808,13 @@
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="R2" t="s">
         <v>94</v>
       </c>
       <c r="S2" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="T2" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Cambios Ajuste Fecha Llamada bienvenida
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6050CCF4-F5A9-49C1-8E2B-8654367EE9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175A9FEA-A177-484F-BBDF-E6529A54F0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -3230,7 +3230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
   <si>
     <t>Cedula</t>
   </si>
@@ -3529,18 +3529,9 @@
     <t>"3183903022"</t>
   </si>
   <si>
-    <t>"13951080"</t>
-  </si>
-  <si>
-    <t>"56530"</t>
-  </si>
-  <si>
     <t>"07/02/2022"</t>
   </si>
   <si>
-    <t>"HERNANDO"</t>
-  </si>
-  <si>
     <t>"P.A COLPENSIONES"</t>
   </si>
   <si>
@@ -3551,6 +3542,18 @@
   </si>
   <si>
     <t>"05/03/2022"</t>
+  </si>
+  <si>
+    <t>"79796"</t>
+  </si>
+  <si>
+    <t>"7425570"</t>
+  </si>
+  <si>
+    <t>"MARIO"</t>
+  </si>
+  <si>
+    <t>"Julio"</t>
   </si>
 </sst>
 </file>
@@ -4198,8 +4201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4320,10 +4323,10 @@
         <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -4347,16 +4350,16 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="N2" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="O2" t="s">
         <v>97</v>
@@ -4374,7 +4377,7 @@
         <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>90</v>
@@ -4392,7 +4395,7 @@
         <v>79</v>
       </c>
       <c r="Z2" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>86</v>
@@ -4633,7 +4636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -4760,13 +4763,13 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
@@ -4808,13 +4811,13 @@
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="R2" t="s">
         <v>94</v>
       </c>
       <c r="S2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="T2" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Cambio calculo remanente para desemboloso retanqueo FINAL
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19939DB2-BEDD-47F1-A97F-EB11C8EDBCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D0AAD0-ABC1-4A41-BAC2-CABA9844EBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1875" windowWidth="20730" windowHeight="11160" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -3230,7 +3230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="109">
   <si>
     <t>Cedula</t>
   </si>
@@ -3451,15 +3451,9 @@
     <t>"1.80"</t>
   </si>
   <si>
-    <t>"1.70"</t>
-  </si>
-  <si>
     <t>"120"</t>
   </si>
   <si>
-    <t>"30"</t>
-  </si>
-  <si>
     <t>FechaRegistro</t>
   </si>
   <si>
@@ -3541,16 +3535,28 @@
     <t>"3183903022"</t>
   </si>
   <si>
-    <t>"07/02/2022"</t>
-  </si>
-  <si>
-    <t>"63275"</t>
-  </si>
-  <si>
-    <t>"13951080"</t>
-  </si>
-  <si>
-    <t>"HERNANDO"</t>
+    <t>"03/03/2022"</t>
+  </si>
+  <si>
+    <t>"99509"</t>
+  </si>
+  <si>
+    <t>"1.71"</t>
+  </si>
+  <si>
+    <t>"Marzo"</t>
+  </si>
+  <si>
+    <t>"7255282"</t>
+  </si>
+  <si>
+    <t>"2036000"</t>
+  </si>
+  <si>
+    <t>"871228"</t>
+  </si>
+  <si>
+    <t>"JAIVER"</t>
   </si>
 </sst>
 </file>
@@ -4199,7 +4205,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4297,54 +4303,54 @@
         <v>31</v>
       </c>
       <c r="V1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="X1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="X1" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="Z1" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="G2" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="K2" t="s">
         <v>42</v>
@@ -4353,49 +4359,49 @@
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="N2" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="O2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="P2" t="s">
         <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S2" t="s">
         <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="W2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA2" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z2" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -4527,10 +4533,10 @@
         <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -4560,7 +4566,7 @@
         <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N2" t="s">
         <v>66</v>
@@ -4740,33 +4746,33 @@
         <v>36</v>
       </c>
       <c r="Y1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA1" t="s">
         <v>80</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>81</v>
       </c>
-      <c r="AA1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>83</v>
-      </c>
       <c r="AC1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AD1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
@@ -4808,22 +4814,22 @@
         <v>22</v>
       </c>
       <c r="Q2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="T2" t="s">
         <v>67</v>
       </c>
       <c r="U2" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="W2" t="s">
         <v>42</v>
@@ -4832,22 +4838,22 @@
         <v>42</v>
       </c>
       <c r="Y2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Z2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC2" t="s">
         <v>84</v>
       </c>
-      <c r="AA2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="AD2" s="15" t="s">
         <v>91</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD2" s="15" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste función SQL; fianza capitalizados y no capitalizados
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataRetanqueo.xlsx
+++ b/src/test/resources/Data/AutomationDataRetanqueo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD566B84-CB83-442E-A3B6-BA139E127F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81215BC7-0478-4A14-B11D-ADCF541A8748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{27C76FE5-7130-4509-9702-8B57384CB331}"/>
   </bookViews>
   <sheets>
     <sheet name="Retanqueo" sheetId="11" r:id="rId1"/>
@@ -4602,36 +4602,12 @@
     <t>"aalvarez@excelcredit.co"</t>
   </si>
   <si>
-    <t>"05/05/1945"</t>
-  </si>
-  <si>
     <t>"3183903022"</t>
   </si>
   <si>
-    <t>"03/03/2022"</t>
-  </si>
-  <si>
-    <t>"99509"</t>
-  </si>
-  <si>
-    <t>"1.71"</t>
-  </si>
-  <si>
     <t>"Marzo"</t>
   </si>
   <si>
-    <t>"7255282"</t>
-  </si>
-  <si>
-    <t>"2036000"</t>
-  </si>
-  <si>
-    <t>"871228"</t>
-  </si>
-  <si>
-    <t>"JAIVER"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Pagaduria</t>
   </si>
   <si>
@@ -5275,6 +5251,30 @@
   </si>
   <si>
     <t>"18/03/2022"</t>
+  </si>
+  <si>
+    <t>"7500000"</t>
+  </si>
+  <si>
+    <t>"200000"</t>
+  </si>
+  <si>
+    <t>"Abril"</t>
+  </si>
+  <si>
+    <t>"25/03/1959"</t>
+  </si>
+  <si>
+    <t>"06/04/2022"</t>
+  </si>
+  <si>
+    <t>"MYRIAM"</t>
+  </si>
+  <si>
+    <t>"95817"</t>
+  </si>
+  <si>
+    <t>"29303804"</t>
   </si>
 </sst>
 </file>
@@ -6239,8 +6239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373B57FB-76BC-4A6C-A0D1-7CDD5BB1EE2F}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6361,16 +6361,16 @@
         <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>306</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>305</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>86</v>
+        <v>203</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>56</v>
@@ -6379,13 +6379,13 @@
         <v>56</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>89</v>
+        <v>299</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>39</v>
+        <v>300</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
         <v>39</v>
@@ -6394,19 +6394,19 @@
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>91</v>
+        <v>304</v>
       </c>
       <c r="N2" t="s">
-        <v>87</v>
+        <v>301</v>
       </c>
       <c r="O2" t="s">
-        <v>82</v>
+        <v>302</v>
       </c>
       <c r="P2" t="s">
         <v>50</v>
       </c>
       <c r="Q2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>81</v>
@@ -6415,7 +6415,7 @@
         <v>28</v>
       </c>
       <c r="T2" t="s">
-        <v>84</v>
+        <v>303</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>71</v>
@@ -6433,7 +6433,7 @@
         <v>60</v>
       </c>
       <c r="Z2" s="12" t="s">
-        <v>84</v>
+        <v>303</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>67</v>
@@ -6948,381 +6948,381 @@
   <sheetData>
     <row r="1" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
+      <c r="J1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" t="s">
+      <c r="K1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
+      <c r="M1" t="s">
         <v>96</v>
       </c>
-      <c r="F1" t="s">
+      <c r="N1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
         <v>98</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" t="s">
         <v>99</v>
       </c>
-      <c r="I1" t="s">
+      <c r="Q1" t="s">
         <v>100</v>
       </c>
-      <c r="J1" t="s">
+      <c r="R1" t="s">
         <v>101</v>
       </c>
-      <c r="K1" t="s">
+      <c r="S1" t="s">
         <v>102</v>
       </c>
-      <c r="L1" t="s">
+      <c r="T1" t="s">
         <v>103</v>
       </c>
-      <c r="M1" t="s">
+      <c r="U1" t="s">
         <v>104</v>
       </c>
-      <c r="N1" t="s">
+      <c r="V1" t="s">
         <v>105</v>
-      </c>
-      <c r="O1" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>108</v>
-      </c>
-      <c r="R1" t="s">
-        <v>109</v>
-      </c>
-      <c r="S1" t="s">
-        <v>110</v>
-      </c>
-      <c r="T1" t="s">
-        <v>111</v>
-      </c>
-      <c r="U1" t="s">
-        <v>112</v>
-      </c>
-      <c r="V1" t="s">
-        <v>113</v>
       </c>
       <c r="W1" t="s">
         <v>5</v>
       </c>
       <c r="X1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF1" t="s">
         <v>114</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AG1" t="s">
         <v>115</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AH1" t="s">
         <v>116</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AI1" t="s">
         <v>117</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>118</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AK1" t="s">
         <v>119</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AL1" t="s">
         <v>120</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AM1" t="s">
         <v>121</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AN1" t="s">
         <v>122</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AO1" t="s">
         <v>123</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AP1" t="s">
         <v>124</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AQ1" t="s">
         <v>125</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AR1" t="s">
         <v>126</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AS1" t="s">
         <v>127</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AT1" t="s">
         <v>128</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AU1" t="s">
         <v>129</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AV1" t="s">
         <v>130</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AW1" t="s">
         <v>131</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AX1" t="s">
         <v>132</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AY1" t="s">
         <v>133</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AZ1" t="s">
         <v>134</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BA1" t="s">
         <v>135</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BB1" t="s">
         <v>136</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BC1" t="s">
         <v>137</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BD1" t="s">
         <v>138</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BE1" t="s">
         <v>139</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BF1" t="s">
         <v>140</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BG1" t="s">
         <v>141</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BH1" t="s">
         <v>142</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BI1" t="s">
         <v>143</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BJ1" t="s">
         <v>144</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BK1" t="s">
         <v>145</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BL1" t="s">
         <v>146</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BM1" t="s">
         <v>147</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BN1" t="s">
         <v>148</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BO1" t="s">
         <v>149</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BP1" t="s">
         <v>150</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BQ1" t="s">
         <v>151</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BR1" t="s">
         <v>152</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BS1" t="s">
         <v>153</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BT1" t="s">
         <v>154</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BU1" t="s">
         <v>155</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BV1" t="s">
         <v>156</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BW1" t="s">
         <v>157</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BX1" t="s">
         <v>158</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BY1" t="s">
         <v>159</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BZ1" t="s">
         <v>160</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CA1" t="s">
         <v>161</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CB1" t="s">
         <v>162</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CC1" t="s">
         <v>163</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CD1" t="s">
         <v>164</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CE1" t="s">
         <v>165</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CF1" t="s">
         <v>166</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CG1" t="s">
         <v>167</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CH1" t="s">
         <v>168</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CI1" t="s">
         <v>169</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CJ1" t="s">
         <v>170</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CK1" t="s">
         <v>171</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CL1" t="s">
         <v>172</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CM1" t="s">
         <v>173</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CN1" t="s">
         <v>174</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CO1" t="s">
         <v>175</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CP1" t="s">
         <v>176</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CQ1" t="s">
         <v>177</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CR1" t="s">
         <v>178</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CS1" t="s">
         <v>179</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CT1" t="s">
         <v>180</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CU1" t="s">
         <v>181</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CV1" t="s">
         <v>182</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CW1" t="s">
         <v>183</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CX1" t="s">
         <v>184</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CY1" t="s">
         <v>185</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CZ1" t="s">
         <v>186</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="DA1" t="s">
         <v>187</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="DB1" t="s">
         <v>188</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="DC1" t="s">
         <v>189</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="DD1" t="s">
         <v>190</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="DE1" t="s">
         <v>191</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="DF1" t="s">
         <v>192</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DG1" t="s">
         <v>193</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DH1" t="s">
         <v>194</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DI1" t="s">
         <v>195</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DJ1" t="s">
         <v>196</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DK1" t="s">
         <v>197</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DL1" t="s">
         <v>198</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DM1" t="s">
         <v>199</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DN1" t="s">
         <v>200</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>201</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>202</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>203</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>204</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>205</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>206</v>
-      </c>
-      <c r="DM1" t="s">
-        <v>207</v>
-      </c>
-      <c r="DN1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>43</v>
@@ -7331,88 +7331,88 @@
         <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="P2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="T2" s="8" t="s">
         <v>39</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="W2" s="15" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="AB2" t="s">
+        <v>217</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>221</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>225</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AK2" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>227</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>228</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>229</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>230</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>231</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>232</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>233</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>234</v>
       </c>
       <c r="AL2" t="s">
         <v>27</v>
@@ -7430,7 +7430,7 @@
         <v>60</v>
       </c>
       <c r="AQ2" s="12" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="AR2" t="s">
         <v>39</v>
@@ -7439,148 +7439,148 @@
         <v>39</v>
       </c>
       <c r="AT2" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>229</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>231</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>233</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>234</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>235</v>
+      </c>
+      <c r="BC2" t="s">
         <v>236</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BD2" t="s">
         <v>237</v>
       </c>
-      <c r="AV2" s="17" t="s">
+      <c r="BE2" t="s">
         <v>238</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BF2" t="s">
         <v>239</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>240</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>241</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>241</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>242</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>243</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>244</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>245</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>246</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>247</v>
       </c>
       <c r="BG2" t="s">
         <v>21</v>
       </c>
       <c r="BH2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="BI2" t="s">
         <v>76</v>
       </c>
       <c r="BJ2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="BK2" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="BL2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="BM2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="BN2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="BO2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="BP2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="BQ2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="BR2" t="s">
         <v>39</v>
       </c>
       <c r="BS2" t="s">
+        <v>248</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>249</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>250</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>251</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>252</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>253</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>254</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>255</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>82</v>
+      </c>
+      <c r="CB2" t="s">
         <v>256</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="CC2" t="s">
         <v>257</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="CD2" t="s">
+        <v>256</v>
+      </c>
+      <c r="CE2" t="s">
         <v>258</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="CF2" t="s">
         <v>259</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="CG2" t="s">
         <v>260</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="CH2" t="s">
         <v>261</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CI2" t="s">
         <v>262</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CJ2" t="s">
         <v>263</v>
       </c>
-      <c r="CA2" t="s">
-        <v>83</v>
-      </c>
-      <c r="CB2" t="s">
+      <c r="CK2" t="s">
         <v>264</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CL2" t="s">
+        <v>256</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>256</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>256</v>
+      </c>
+      <c r="CO2" t="s">
         <v>265</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>264</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>266</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>267</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>268</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>269</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>270</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>271</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>272</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>264</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>264</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>264</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>273</v>
       </c>
       <c r="CP2" t="s">
         <v>75</v>
@@ -7592,70 +7592,70 @@
         <v>50</v>
       </c>
       <c r="CS2" t="s">
+        <v>266</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>267</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>268</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>269</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>256</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>270</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>271</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>272</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>273</v>
+      </c>
+      <c r="DB2" t="s">
         <v>274</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="DC2" t="s">
         <v>275</v>
       </c>
-      <c r="CU2" t="s">
+      <c r="DD2" t="s">
         <v>276</v>
       </c>
-      <c r="CV2" t="s">
+      <c r="DE2" t="s">
         <v>277</v>
       </c>
-      <c r="CW2" t="s">
-        <v>264</v>
-      </c>
-      <c r="CX2" t="s">
+      <c r="DF2" t="s">
         <v>278</v>
       </c>
-      <c r="CY2" t="s">
+      <c r="DG2" t="s">
         <v>279</v>
       </c>
-      <c r="CZ2" t="s">
+      <c r="DH2" t="s">
         <v>280</v>
       </c>
-      <c r="DA2" t="s">
+      <c r="DI2" t="s">
         <v>281</v>
       </c>
-      <c r="DB2" t="s">
+      <c r="DJ2" t="s">
         <v>282</v>
       </c>
-      <c r="DC2" t="s">
+      <c r="DK2" t="s">
         <v>283</v>
       </c>
-      <c r="DD2" t="s">
+      <c r="DL2" t="s">
+        <v>256</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>288</v>
+      </c>
+      <c r="DN2" t="s">
         <v>284</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>285</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>286</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>287</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>288</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>289</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>290</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>291</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>264</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>296</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -7731,7 +7731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4941B7E2-706E-4D94-84AC-BEDA7D2028C7}">
   <dimension ref="A1:DN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -7764,381 +7764,381 @@
   <sheetData>
     <row r="1" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
+      <c r="J1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" t="s">
+      <c r="K1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
+      <c r="M1" t="s">
         <v>96</v>
       </c>
-      <c r="F1" t="s">
+      <c r="N1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
         <v>98</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" t="s">
         <v>99</v>
       </c>
-      <c r="I1" t="s">
+      <c r="Q1" t="s">
         <v>100</v>
       </c>
-      <c r="J1" t="s">
+      <c r="R1" t="s">
         <v>101</v>
       </c>
-      <c r="K1" t="s">
+      <c r="S1" t="s">
         <v>102</v>
       </c>
-      <c r="L1" t="s">
+      <c r="T1" t="s">
         <v>103</v>
       </c>
-      <c r="M1" t="s">
+      <c r="U1" t="s">
         <v>104</v>
       </c>
-      <c r="N1" t="s">
+      <c r="V1" t="s">
         <v>105</v>
-      </c>
-      <c r="O1" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>108</v>
-      </c>
-      <c r="R1" t="s">
-        <v>109</v>
-      </c>
-      <c r="S1" t="s">
-        <v>110</v>
-      </c>
-      <c r="T1" t="s">
-        <v>111</v>
-      </c>
-      <c r="U1" t="s">
-        <v>112</v>
-      </c>
-      <c r="V1" t="s">
-        <v>113</v>
       </c>
       <c r="W1" t="s">
         <v>5</v>
       </c>
       <c r="X1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF1" t="s">
         <v>114</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AG1" t="s">
         <v>115</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AH1" t="s">
         <v>116</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AI1" t="s">
         <v>117</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>118</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AK1" t="s">
         <v>119</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AL1" t="s">
         <v>120</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AM1" t="s">
         <v>121</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AN1" t="s">
         <v>122</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AO1" t="s">
         <v>123</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AP1" t="s">
         <v>124</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AQ1" t="s">
         <v>125</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AR1" t="s">
         <v>126</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AS1" t="s">
         <v>127</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AT1" t="s">
         <v>128</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AU1" t="s">
         <v>129</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AV1" t="s">
         <v>130</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AW1" t="s">
         <v>131</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AX1" t="s">
         <v>132</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AY1" t="s">
         <v>133</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AZ1" t="s">
         <v>134</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BA1" t="s">
         <v>135</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BB1" t="s">
         <v>136</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BC1" t="s">
         <v>137</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BD1" t="s">
         <v>138</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BE1" t="s">
         <v>139</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BF1" t="s">
         <v>140</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BG1" t="s">
         <v>141</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BH1" t="s">
         <v>142</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BI1" t="s">
         <v>143</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BJ1" t="s">
         <v>144</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BK1" t="s">
         <v>145</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BL1" t="s">
         <v>146</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BM1" t="s">
         <v>147</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BN1" t="s">
         <v>148</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BO1" t="s">
         <v>149</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BP1" t="s">
         <v>150</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BQ1" t="s">
         <v>151</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BR1" t="s">
         <v>152</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BS1" t="s">
         <v>153</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BT1" t="s">
         <v>154</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BU1" t="s">
         <v>155</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BV1" t="s">
         <v>156</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BW1" t="s">
         <v>157</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BX1" t="s">
         <v>158</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BY1" t="s">
         <v>159</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BZ1" t="s">
         <v>160</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CA1" t="s">
         <v>161</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CB1" t="s">
         <v>162</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CC1" t="s">
         <v>163</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CD1" t="s">
         <v>164</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CE1" t="s">
         <v>165</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CF1" t="s">
         <v>166</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CG1" t="s">
         <v>167</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CH1" t="s">
         <v>168</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CI1" t="s">
         <v>169</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CJ1" t="s">
         <v>170</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CK1" t="s">
         <v>171</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CL1" t="s">
         <v>172</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CM1" t="s">
         <v>173</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CN1" t="s">
         <v>174</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CO1" t="s">
         <v>175</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CP1" t="s">
         <v>176</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CQ1" t="s">
         <v>177</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CR1" t="s">
         <v>178</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CS1" t="s">
         <v>179</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CT1" t="s">
         <v>180</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CU1" t="s">
         <v>181</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CV1" t="s">
         <v>182</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CW1" t="s">
         <v>183</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CX1" t="s">
         <v>184</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CY1" t="s">
         <v>185</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CZ1" t="s">
         <v>186</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="DA1" t="s">
         <v>187</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="DB1" t="s">
         <v>188</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="DC1" t="s">
         <v>189</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="DD1" t="s">
         <v>190</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="DE1" t="s">
         <v>191</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="DF1" t="s">
         <v>192</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DG1" t="s">
         <v>193</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DH1" t="s">
         <v>194</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DI1" t="s">
         <v>195</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DJ1" t="s">
         <v>196</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DK1" t="s">
         <v>197</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DL1" t="s">
         <v>198</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DM1" t="s">
         <v>199</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DN1" t="s">
         <v>200</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>201</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>202</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>203</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>204</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>205</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>206</v>
-      </c>
-      <c r="DM1" t="s">
-        <v>207</v>
-      </c>
-      <c r="DN1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>56</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>43</v>
@@ -8147,88 +8147,88 @@
         <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="P2" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="V2" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="W2" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y2" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="P2" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="AB2" t="s">
+        <v>217</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>221</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>225</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AK2" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>227</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>228</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>229</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>230</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>231</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>232</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>233</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>234</v>
       </c>
       <c r="AL2" t="s">
         <v>50</v>
@@ -8246,7 +8246,7 @@
         <v>60</v>
       </c>
       <c r="AQ2" s="12" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="AR2" t="s">
         <v>39</v>
@@ -8255,148 +8255,148 @@
         <v>39</v>
       </c>
       <c r="AT2" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>229</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>231</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>233</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>234</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>235</v>
+      </c>
+      <c r="BC2" t="s">
         <v>236</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BD2" t="s">
         <v>237</v>
       </c>
-      <c r="AV2" s="17" t="s">
+      <c r="BE2" t="s">
         <v>238</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BF2" t="s">
         <v>239</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>303</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>241</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>241</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>242</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>243</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>244</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>245</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>246</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>247</v>
       </c>
       <c r="BG2" t="s">
         <v>21</v>
       </c>
       <c r="BH2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="BI2" t="s">
         <v>76</v>
       </c>
       <c r="BJ2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="BK2" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="BL2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="BM2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="BN2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="BO2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="BP2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="BQ2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="BR2" t="s">
         <v>39</v>
       </c>
       <c r="BS2" t="s">
+        <v>248</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>249</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>250</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>251</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>252</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>253</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>254</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>255</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>82</v>
+      </c>
+      <c r="CB2" t="s">
         <v>256</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="CC2" t="s">
         <v>257</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="CD2" t="s">
+        <v>256</v>
+      </c>
+      <c r="CE2" t="s">
         <v>258</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="CF2" t="s">
         <v>259</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="CG2" t="s">
         <v>260</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="CH2" t="s">
         <v>261</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CI2" t="s">
         <v>262</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CJ2" t="s">
         <v>263</v>
       </c>
-      <c r="CA2" t="s">
-        <v>83</v>
-      </c>
-      <c r="CB2" t="s">
+      <c r="CK2" t="s">
         <v>264</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CL2" t="s">
+        <v>256</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>256</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>256</v>
+      </c>
+      <c r="CO2" t="s">
         <v>265</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>264</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>266</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>267</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>268</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>269</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>270</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>271</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>272</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>264</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>264</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>264</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>273</v>
       </c>
       <c r="CP2" t="s">
         <v>75</v>
@@ -8408,70 +8408,70 @@
         <v>50</v>
       </c>
       <c r="CS2" t="s">
+        <v>266</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>267</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>268</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>269</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>296</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>270</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>271</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>272</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>273</v>
+      </c>
+      <c r="DB2" t="s">
         <v>274</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="DC2" t="s">
         <v>275</v>
       </c>
-      <c r="CU2" t="s">
+      <c r="DD2" t="s">
         <v>276</v>
       </c>
-      <c r="CV2" t="s">
+      <c r="DE2" t="s">
         <v>277</v>
       </c>
-      <c r="CW2" t="s">
-        <v>304</v>
-      </c>
-      <c r="CX2" t="s">
+      <c r="DF2" t="s">
         <v>278</v>
       </c>
-      <c r="CY2" t="s">
+      <c r="DG2" t="s">
         <v>279</v>
       </c>
-      <c r="CZ2" t="s">
+      <c r="DH2" t="s">
         <v>280</v>
       </c>
-      <c r="DA2" t="s">
+      <c r="DI2" t="s">
         <v>281</v>
       </c>
-      <c r="DB2" t="s">
+      <c r="DJ2" t="s">
         <v>282</v>
       </c>
-      <c r="DC2" t="s">
+      <c r="DK2" t="s">
         <v>283</v>
       </c>
-      <c r="DD2" t="s">
+      <c r="DL2" t="s">
+        <v>256</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>297</v>
+      </c>
+      <c r="DN2" t="s">
         <v>284</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>285</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>286</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>287</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>288</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>289</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>290</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>291</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>264</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>305</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>